<commit_message>
up to chapter 3, for 2ed week 20210
</commit_message>
<xml_diff>
--- a/Chap2_Assett_Selling/data/asset_selling_policy_parameters_edit.xlsx
+++ b/Chap2_Assett_Selling/data/asset_selling_policy_parameters_edit.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t xml:space="preserve">1)</t>
   </si>
@@ -68,6 +68,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">The possible outcomes for the bias are {'Up','Neutral','Down'}. The bias is part of the state variable. The probability of bias_{t+1} being equal to Up', 'Neutral' or 'Down' depends on the bias_{t}. Use '</t>
     </r>
@@ -78,6 +79,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Sheet4'</t>
     </r>
@@ -87,6 +89,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> to set this probabiliy matrix</t>
     </r>
@@ -98,6 +101,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">The possible outcomes for the mean are  {UpStep, 0, DownStep} depending if the bias is  'Up',' Neutral' or 'Down', respectively. Use '</t>
     </r>
@@ -108,6 +112,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Sheet3</t>
     </r>
@@ -117,6 +122,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">' to set up these values. </t>
     </r>
@@ -126,6 +132,9 @@
   </si>
   <si>
     <t xml:space="preserve">After setting up the parameters and saving this spreadsheet, just run  'AssetSellingDriverScript'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">policy</t>
   </si>
   <si>
     <t xml:space="preserve">param1</t>
@@ -208,12 +217,13 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -232,134 +242,22 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF0000EE"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -367,23 +265,8 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -407,57 +290,6 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -473,91 +305,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000EE"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -664,7 +419,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -673,18 +428,21 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>16</v>
+      </c>
       <c r="B1" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>2</v>
@@ -695,7 +453,7 @@
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>4</v>
@@ -708,7 +466,7 @@
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>0</v>
@@ -750,19 +508,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -800,8 +558,8 @@
   </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -813,39 +571,39 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>40</v>
@@ -857,7 +615,7 @@
         <v>16</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>1</v>
@@ -869,7 +627,7 @@
         <v>2</v>
       </c>
       <c r="I2" s="0" t="n">
-        <v>10000</v>
+        <v>10</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>40</v>
@@ -893,7 +651,7 @@
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -904,21 +662,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>36</v>
-      </c>
       <c r="C1" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.9</v>
@@ -932,7 +690,7 @@
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.2</v>
@@ -946,7 +704,7 @@
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
the begining of chapter 4
</commit_message>
<xml_diff>
--- a/Chap2_Assett_Selling/data/asset_selling_policy_parameters_edit.xlsx
+++ b/Chap2_Assett_Selling/data/asset_selling_policy_parameters_edit.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -495,8 +495,8 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -525,16 +525,16 @@
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>0.01</v>
+        <v>18</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>0.005</v>
@@ -558,7 +558,7 @@
   </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>

</xml_diff>